<commit_message>
Adicionado Coluna Desconto unitário
</commit_message>
<xml_diff>
--- a/01-Produtos.xlsx
+++ b/01-Produtos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafae\Meu Drive (mz.tears.of.time@gmail.com)\Front - Back\Curso-003\001 - Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DC8017-D78D-4C26-9D20-149EC9D42681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E145AD-92F5-4844-8B9F-2453FEA24D44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="23070" windowHeight="11505" activeTab="2" xr2:uid="{D1AB1EC9-71FA-412A-B8FE-746C2A8742A3}"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="23070" windowHeight="11505" activeTab="3" xr2:uid="{D1AB1EC9-71FA-412A-B8FE-746C2A8742A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="36">
   <si>
     <t>Bermuda</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Desconto</t>
   </si>
   <si>
-    <t>Valor do Desconto</t>
-  </si>
-  <si>
     <t>Qtde</t>
   </si>
   <si>
@@ -143,6 +140,18 @@
   </si>
   <si>
     <t>Layout Rapido</t>
+  </si>
+  <si>
+    <t>Preço c/ Desconto</t>
+  </si>
+  <si>
+    <t>Valor do DescontoTotal</t>
+  </si>
+  <si>
+    <t>Preço C/ Desconto</t>
+  </si>
+  <si>
+    <t>Valor Desconto Total</t>
   </si>
 </sst>
 </file>
@@ -644,6 +653,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -653,15 +664,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -677,6 +690,9 @@
       <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -687,7 +703,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
@@ -829,27 +844,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="4"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="63500">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="25000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -1856,7 +1851,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Rafa RPG" refreshedDate="45465.701305092596" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="20" xr:uid="{84BDBEC6-9621-4193-B194-892E94979D5B}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:G23" sheet="Produtos"/>
+    <worksheetSource ref="A3:H23" sheet="Produtos"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="Produtos" numFmtId="0">
@@ -2086,7 +2081,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBDBE488-3B1B-40A8-A9CB-84B68462659D}" name="Tabela dinâmica17" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EBDBE488-3B1B-40A8-A9CB-84B68462659D}" name="Tabela dinâmica17" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A1:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -2216,19 +2211,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307A5C2F-2ED0-4132-A755-33287BFED071}" name="Tabela3" displayName="Tabela3" ref="A3:G24" totalsRowCount="1" headerRowDxfId="12">
-  <autoFilter ref="A3:G23" xr:uid="{DD085341-96D5-448C-ACB6-B9B20E85FF90}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B3BB856A-94C5-4DBF-A426-729A6175E54C}" name="Produtos" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{57EE2957-B617-4F1F-99BF-A943B55BA5EF}" name="Tamanho" dataDxfId="11" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{3EC27319-A449-4A3F-BC2A-10D434BF2077}" name="Categoria" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A4DC478E-BD53-452B-A86C-6BBB49DC23EB}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DFA69D81-EF82-4249-9B1C-2E6D4A2555E8}" name="Qtde" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{D884E988-6577-4BED-AA7D-358FDCE039D6}" name="Valor Total" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307A5C2F-2ED0-4132-A755-33287BFED071}" name="Tabela3" displayName="Tabela3" ref="A3:H24" totalsRowCount="1" headerRowDxfId="14">
+  <autoFilter ref="A3:H23" xr:uid="{DD085341-96D5-448C-ACB6-B9B20E85FF90}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B3BB856A-94C5-4DBF-A426-729A6175E54C}" name="Produtos" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{57EE2957-B617-4F1F-99BF-A943B55BA5EF}" name="Tamanho" dataDxfId="13" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{3EC27319-A449-4A3F-BC2A-10D434BF2077}" name="Categoria" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A4DC478E-BD53-452B-A86C-6BBB49DC23EB}" name="Preço Unitário" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{EE3B769A-D813-4769-948F-240A6BB92138}" name="Preço C/ Desconto" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="4">
+      <calculatedColumnFormula>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{DFA69D81-EF82-4249-9B1C-2E6D4A2555E8}" name="Qtde" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{D884E988-6577-4BED-AA7D-358FDCE039D6}" name="Valor Total" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2">
       <calculatedColumnFormula>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FC1C4EC2-D807-40BF-ABDA-2A64A12A1AC9}" name="Valor do Desconto" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="0">
-      <calculatedColumnFormula>Tabela3[[#This Row],[Valor Total]]*$I$4</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{FC1C4EC2-D807-40BF-ABDA-2A64A12A1AC9}" name="Valor Desconto Total" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+      <calculatedColumnFormula>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2532,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114E7D90-B6FA-4067-AF2F-B7057AE08EDA}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" activeCellId="1" sqref="A3:A23 E3:E23"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,24 +2542,26 @@
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2569,8 +2569,9 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
@@ -2584,19 +2585,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="32" t="s">
+      <c r="H3" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
@@ -2609,22 +2613,26 @@
       <c r="D4" s="19">
         <v>25.9</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
+        <f>D4-(D4*$J$4)</f>
+        <v>24.604999999999997</v>
+      </c>
+      <c r="F4" s="20">
         <v>12</v>
       </c>
-      <c r="F4" s="19">
-        <f>D4*E4</f>
+      <c r="G4" s="19">
+        <f>D4*F4</f>
         <v>310.79999999999995</v>
       </c>
-      <c r="G4" s="19">
-        <f>F4*$I$4</f>
-        <v>15.54</v>
-      </c>
-      <c r="I4" s="33">
+      <c r="H4" s="19">
+        <f>E4*F4</f>
+        <v>295.26</v>
+      </c>
+      <c r="J4" s="33">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -2637,19 +2645,23 @@
       <c r="D5" s="18">
         <v>29.9</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
+        <f t="shared" ref="E5:E23" si="0">D5-(D5*$J$4)</f>
+        <v>28.404999999999998</v>
+      </c>
+      <c r="F5" s="21">
         <v>10</v>
       </c>
-      <c r="F5" s="19">
-        <f t="shared" ref="F5:F23" si="0">D5*E5</f>
+      <c r="G5" s="19">
+        <f>D5*F5</f>
         <v>299</v>
       </c>
-      <c r="G5" s="19">
-        <f t="shared" ref="G5:G23" si="1">F5*$I$4</f>
-        <v>14.950000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="19">
+        <f t="shared" ref="H5:H23" si="1">E5*F5</f>
+        <v>284.04999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -2662,19 +2674,23 @@
       <c r="D6" s="18">
         <v>32.9</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
+        <f t="shared" si="0"/>
+        <v>31.254999999999999</v>
+      </c>
+      <c r="F6" s="21">
         <v>6</v>
       </c>
-      <c r="F6" s="19">
-        <f t="shared" si="0"/>
+      <c r="G6" s="19">
+        <f>D6*F6</f>
         <v>197.39999999999998</v>
       </c>
-      <c r="G6" s="19">
+      <c r="H6" s="19">
         <f t="shared" si="1"/>
-        <v>9.8699999999999992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>187.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -2687,19 +2703,23 @@
       <c r="D7" s="18">
         <v>399.9</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
+        <f t="shared" si="0"/>
+        <v>379.90499999999997</v>
+      </c>
+      <c r="F7" s="21">
         <v>3</v>
       </c>
-      <c r="F7" s="19">
-        <f t="shared" si="0"/>
+      <c r="G7" s="19">
+        <f>D7*F7</f>
         <v>1199.6999999999998</v>
       </c>
-      <c r="G7" s="19">
+      <c r="H7" s="19">
         <f t="shared" si="1"/>
-        <v>59.984999999999992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1139.7149999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>17</v>
       </c>
@@ -2712,19 +2732,23 @@
       <c r="D8" s="18">
         <v>249.9</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
+        <f t="shared" si="0"/>
+        <v>237.405</v>
+      </c>
+      <c r="F8" s="21">
         <v>1</v>
       </c>
-      <c r="F8" s="19">
-        <f t="shared" si="0"/>
+      <c r="G8" s="19">
+        <f>D8*F8</f>
         <v>249.9</v>
       </c>
-      <c r="G8" s="19">
+      <c r="H8" s="19">
         <f t="shared" si="1"/>
-        <v>12.495000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>237.405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
@@ -2737,19 +2761,23 @@
       <c r="D9" s="18">
         <v>259.89999999999998</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
+        <f t="shared" si="0"/>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="19">
-        <f t="shared" si="0"/>
+      <c r="G9" s="19">
+        <f>D9*F9</f>
         <v>519.79999999999995</v>
       </c>
-      <c r="G9" s="19">
+      <c r="H9" s="19">
         <f t="shared" si="1"/>
-        <v>25.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>493.80999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -2762,19 +2790,23 @@
       <c r="D10" s="18">
         <v>299.89999999999998</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
+        <f t="shared" si="0"/>
+        <v>284.90499999999997</v>
+      </c>
+      <c r="F10" s="21">
         <v>1</v>
       </c>
-      <c r="F10" s="19">
-        <f t="shared" si="0"/>
+      <c r="G10" s="19">
+        <f>D10*F10</f>
         <v>299.89999999999998</v>
       </c>
-      <c r="G10" s="19">
+      <c r="H10" s="19">
         <f t="shared" si="1"/>
-        <v>14.994999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>284.90499999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
@@ -2787,19 +2819,23 @@
       <c r="D11" s="18">
         <v>85.9</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
+        <f t="shared" si="0"/>
+        <v>81.605000000000004</v>
+      </c>
+      <c r="F11" s="21">
         <v>8</v>
       </c>
-      <c r="F11" s="19">
-        <f t="shared" si="0"/>
+      <c r="G11" s="19">
+        <f>D11*F11</f>
         <v>687.2</v>
       </c>
-      <c r="G11" s="19">
+      <c r="H11" s="19">
         <f t="shared" si="1"/>
-        <v>34.360000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>652.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -2812,19 +2848,23 @@
       <c r="D12" s="18">
         <v>89.9</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
+        <f t="shared" si="0"/>
+        <v>85.405000000000001</v>
+      </c>
+      <c r="F12" s="21">
         <v>5</v>
       </c>
-      <c r="F12" s="19">
-        <f t="shared" si="0"/>
+      <c r="G12" s="19">
+        <f>D12*F12</f>
         <v>449.5</v>
       </c>
-      <c r="G12" s="19">
+      <c r="H12" s="19">
         <f t="shared" si="1"/>
-        <v>22.475000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>427.02499999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>18</v>
       </c>
@@ -2837,19 +2877,23 @@
       <c r="D13" s="18">
         <v>92.9</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="19">
+        <f t="shared" si="0"/>
+        <v>88.25500000000001</v>
+      </c>
+      <c r="F13" s="21">
         <v>6</v>
       </c>
-      <c r="F13" s="19">
-        <f t="shared" si="0"/>
+      <c r="G13" s="19">
+        <f>D13*F13</f>
         <v>557.40000000000009</v>
       </c>
-      <c r="G13" s="19">
+      <c r="H13" s="19">
         <f t="shared" si="1"/>
-        <v>27.870000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>529.53000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
@@ -2862,19 +2906,23 @@
       <c r="D14" s="18">
         <v>149.9</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="19">
+        <f t="shared" si="0"/>
+        <v>142.405</v>
+      </c>
+      <c r="F14" s="21">
         <v>2</v>
       </c>
-      <c r="F14" s="19">
-        <f t="shared" si="0"/>
+      <c r="G14" s="19">
+        <f>D14*F14</f>
         <v>299.8</v>
       </c>
-      <c r="G14" s="19">
+      <c r="H14" s="19">
         <f t="shared" si="1"/>
-        <v>14.990000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>284.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>0</v>
       </c>
@@ -2887,19 +2935,23 @@
       <c r="D15" s="18">
         <v>65.900000000000006</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="19">
+        <f t="shared" si="0"/>
+        <v>62.605000000000004</v>
+      </c>
+      <c r="F15" s="21">
         <v>12</v>
       </c>
-      <c r="F15" s="19">
-        <f t="shared" si="0"/>
+      <c r="G15" s="19">
+        <f>D15*F15</f>
         <v>790.80000000000007</v>
       </c>
-      <c r="G15" s="19">
+      <c r="H15" s="19">
         <f t="shared" si="1"/>
-        <v>39.540000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>751.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
@@ -2912,19 +2964,23 @@
       <c r="D16" s="18">
         <v>69.900000000000006</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="19">
+        <f t="shared" si="0"/>
+        <v>66.405000000000001</v>
+      </c>
+      <c r="F16" s="21">
         <v>15</v>
       </c>
-      <c r="F16" s="19">
-        <f t="shared" si="0"/>
+      <c r="G16" s="19">
+        <f>D16*F16</f>
         <v>1048.5</v>
       </c>
-      <c r="G16" s="19">
+      <c r="H16" s="19">
         <f t="shared" si="1"/>
-        <v>52.425000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>996.07500000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
@@ -2937,19 +2993,23 @@
       <c r="D17" s="18">
         <v>70.900000000000006</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="19">
+        <f t="shared" si="0"/>
+        <v>67.355000000000004</v>
+      </c>
+      <c r="F17" s="21">
         <v>13</v>
       </c>
-      <c r="F17" s="19">
-        <f t="shared" si="0"/>
+      <c r="G17" s="19">
+        <f>D17*F17</f>
         <v>921.7</v>
       </c>
-      <c r="G17" s="19">
+      <c r="H17" s="19">
         <f t="shared" si="1"/>
-        <v>46.085000000000008</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>875.61500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>1</v>
       </c>
@@ -2962,19 +3022,23 @@
       <c r="D18" s="18">
         <v>199.9</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="19">
+        <f t="shared" si="0"/>
+        <v>189.905</v>
+      </c>
+      <c r="F18" s="21">
         <v>2</v>
       </c>
-      <c r="F18" s="19">
-        <f t="shared" si="0"/>
+      <c r="G18" s="19">
+        <f>D18*F18</f>
         <v>399.8</v>
       </c>
-      <c r="G18" s="19">
+      <c r="H18" s="19">
         <f t="shared" si="1"/>
-        <v>19.990000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>379.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>1</v>
       </c>
@@ -2987,19 +3051,23 @@
       <c r="D19" s="18">
         <v>249.9</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="19">
+        <f t="shared" si="0"/>
+        <v>237.405</v>
+      </c>
+      <c r="F19" s="21">
         <v>1</v>
       </c>
-      <c r="F19" s="19">
-        <f t="shared" si="0"/>
+      <c r="G19" s="19">
+        <f>D19*F19</f>
         <v>249.9</v>
       </c>
-      <c r="G19" s="19">
+      <c r="H19" s="19">
         <f t="shared" si="1"/>
-        <v>12.495000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>237.405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>1</v>
       </c>
@@ -3012,19 +3080,23 @@
       <c r="D20" s="18">
         <v>259.89999999999998</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="19">
+        <f t="shared" si="0"/>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F20" s="21">
         <v>0</v>
       </c>
-      <c r="F20" s="19">
-        <f t="shared" si="0"/>
+      <c r="G20" s="19">
+        <f>D20*F20</f>
         <v>0</v>
       </c>
-      <c r="G20" s="19">
+      <c r="H20" s="19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>2</v>
       </c>
@@ -3037,19 +3109,23 @@
       <c r="D21" s="18">
         <v>259.89999999999998</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="19">
+        <f t="shared" si="0"/>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F21" s="21">
         <v>1</v>
       </c>
-      <c r="F21" s="19">
-        <f t="shared" si="0"/>
+      <c r="G21" s="19">
+        <f>D21*F21</f>
         <v>259.89999999999998</v>
       </c>
-      <c r="G21" s="19">
+      <c r="H21" s="19">
         <f t="shared" si="1"/>
-        <v>12.994999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>246.90499999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>3</v>
       </c>
@@ -3062,19 +3138,23 @@
       <c r="D22" s="18">
         <v>39.9</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="19">
+        <f t="shared" si="0"/>
+        <v>37.905000000000001</v>
+      </c>
+      <c r="F22" s="21">
         <v>11</v>
       </c>
-      <c r="F22" s="19">
-        <f t="shared" si="0"/>
+      <c r="G22" s="19">
+        <f>D22*F22</f>
         <v>438.9</v>
       </c>
-      <c r="G22" s="19">
+      <c r="H22" s="19">
         <f t="shared" si="1"/>
-        <v>21.945</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>416.95500000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>4</v>
       </c>
@@ -3087,19 +3167,23 @@
       <c r="D23" s="23">
         <v>49.9</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="19">
+        <f t="shared" si="0"/>
+        <v>47.405000000000001</v>
+      </c>
+      <c r="F23" s="24">
         <v>21</v>
       </c>
-      <c r="F23" s="25">
-        <f t="shared" si="0"/>
+      <c r="G23" s="25">
+        <f>D23*F23</f>
         <v>1047.8999999999999</v>
       </c>
-      <c r="G23" s="19">
+      <c r="H23" s="19">
         <f t="shared" si="1"/>
-        <v>52.394999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>995.505</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -3107,39 +3191,45 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="34" t="s">
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="26">
         <f>SUM(D4:D23)</f>
         <v>2983.0000000000009</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="28">
         <f>SUM(E4:E23)</f>
+        <v>2833.8500000000004</v>
+      </c>
+      <c r="F25" s="27">
+        <f>SUM(F4:F23)</f>
         <v>132</v>
-      </c>
-      <c r="F25" s="28">
-        <f>SUM(F4:F23)</f>
-        <v>10227.799999999999</v>
       </c>
       <c r="G25" s="28">
         <f>SUM(G4:G23)</f>
-        <v>511.39000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10227.799999999999</v>
+      </c>
+      <c r="H25" s="28">
+        <f>SUM(H4:H23)</f>
+        <v>9716.41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D27" s="22"/>
-      <c r="F27" s="22"/>
+      <c r="E27" s="22"/>
       <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3150,7 +3240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9AE3DD-79DC-4C6F-86EE-0CA56541D5E9}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -3161,51 +3251,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38">
+      <c r="B2" s="35">
         <v>40</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="38">
+      <c r="B3" s="35">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="35">
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="35">
         <v>19</v>
       </c>
     </row>
@@ -3213,7 +3303,7 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="38">
+      <c r="B6" s="35">
         <v>28</v>
       </c>
     </row>
@@ -3221,7 +3311,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7" s="35">
         <v>21</v>
       </c>
     </row>
@@ -3229,7 +3319,7 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="35">
         <v>4</v>
       </c>
     </row>
@@ -3237,7 +3327,7 @@
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="38">
+      <c r="B9" s="35">
         <v>3</v>
       </c>
     </row>
@@ -3245,7 +3335,7 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="38">
+      <c r="B10" s="35">
         <v>3</v>
       </c>
     </row>
@@ -3253,7 +3343,7 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="38">
+      <c r="B11" s="35">
         <v>2</v>
       </c>
     </row>
@@ -3267,10 +3357,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E3" activeCellId="1" sqref="A3:A23 E3:E23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,24 +3369,25 @@
     <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-    </row>
-    <row r="2" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -3304,8 +3395,9 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -3319,19 +3411,22 @@
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="30" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3344,22 +3439,26 @@
       <c r="D4" s="22">
         <v>25.9</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>24.604999999999997</v>
+      </c>
+      <c r="F4" s="1">
         <v>12</v>
       </c>
-      <c r="F4" s="22">
+      <c r="G4" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>310.79999999999995</v>
       </c>
-      <c r="G4" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>15.54</v>
-      </c>
-      <c r="I4" s="31">
+      <c r="H4" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>295.26</v>
+      </c>
+      <c r="J4" s="31">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3372,19 +3471,23 @@
       <c r="D5" s="22">
         <v>29.9</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>28.404999999999998</v>
+      </c>
+      <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="F5" s="22">
+      <c r="G5" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>299</v>
       </c>
-      <c r="G5" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>14.950000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>284.04999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3397,19 +3500,23 @@
       <c r="D6" s="22">
         <v>32.9</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>31.254999999999999</v>
+      </c>
+      <c r="F6" s="1">
         <v>6</v>
       </c>
-      <c r="F6" s="22">
+      <c r="G6" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>197.39999999999998</v>
       </c>
-      <c r="G6" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>9.8699999999999992</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>187.53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -3422,19 +3529,23 @@
       <c r="D7" s="22">
         <v>399.9</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>379.90499999999997</v>
+      </c>
+      <c r="F7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="22">
+      <c r="G7" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>1199.6999999999998</v>
       </c>
-      <c r="G7" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>59.984999999999992</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>1139.7149999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -3447,19 +3558,23 @@
       <c r="D8" s="22">
         <v>249.9</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>237.405</v>
+      </c>
+      <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="F8" s="22">
+      <c r="G8" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>249.9</v>
       </c>
-      <c r="G8" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>12.495000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>237.405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -3472,19 +3587,23 @@
       <c r="D9" s="22">
         <v>259.89999999999998</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="22">
+      <c r="G9" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>519.79999999999995</v>
       </c>
-      <c r="G9" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>25.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>493.80999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -3497,19 +3616,23 @@
       <c r="D10" s="22">
         <v>299.89999999999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>284.90499999999997</v>
+      </c>
+      <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="22">
+      <c r="G10" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>299.89999999999998</v>
       </c>
-      <c r="G10" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>14.994999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>284.90499999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3522,19 +3645,23 @@
       <c r="D11" s="22">
         <v>85.9</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>81.605000000000004</v>
+      </c>
+      <c r="F11" s="1">
         <v>8</v>
       </c>
-      <c r="F11" s="22">
+      <c r="G11" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>687.2</v>
       </c>
-      <c r="G11" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>34.360000000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>652.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -3547,19 +3674,23 @@
       <c r="D12" s="22">
         <v>89.9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>85.405000000000001</v>
+      </c>
+      <c r="F12" s="1">
         <v>5</v>
       </c>
-      <c r="F12" s="22">
+      <c r="G12" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>449.5</v>
       </c>
-      <c r="G12" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>22.475000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>427.02499999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3572,19 +3703,23 @@
       <c r="D13" s="22">
         <v>92.9</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>88.25500000000001</v>
+      </c>
+      <c r="F13" s="1">
         <v>6</v>
       </c>
-      <c r="F13" s="22">
+      <c r="G13" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>557.40000000000009</v>
       </c>
-      <c r="G13" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>27.870000000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>529.53000000000009</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -3597,19 +3732,23 @@
       <c r="D14" s="22">
         <v>149.9</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>142.405</v>
+      </c>
+      <c r="F14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="G14" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>299.8</v>
       </c>
-      <c r="G14" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>14.990000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>284.81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -3622,19 +3761,23 @@
       <c r="D15" s="22">
         <v>65.900000000000006</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>62.605000000000004</v>
+      </c>
+      <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="F15" s="22">
+      <c r="G15" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>790.80000000000007</v>
       </c>
-      <c r="G15" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>39.540000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>751.26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -3647,19 +3790,23 @@
       <c r="D16" s="22">
         <v>69.900000000000006</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>66.405000000000001</v>
+      </c>
+      <c r="F16" s="1">
         <v>15</v>
       </c>
-      <c r="F16" s="22">
+      <c r="G16" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>1048.5</v>
       </c>
-      <c r="G16" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>52.425000000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>996.07500000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -3672,19 +3819,23 @@
       <c r="D17" s="22">
         <v>70.900000000000006</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>67.355000000000004</v>
+      </c>
+      <c r="F17" s="1">
         <v>13</v>
       </c>
-      <c r="F17" s="22">
+      <c r="G17" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>921.7</v>
       </c>
-      <c r="G17" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>46.085000000000008</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>875.61500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3697,19 +3848,23 @@
       <c r="D18" s="22">
         <v>199.9</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>189.905</v>
+      </c>
+      <c r="F18" s="1">
         <v>2</v>
       </c>
-      <c r="F18" s="22">
+      <c r="G18" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>399.8</v>
       </c>
-      <c r="G18" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>19.990000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>379.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3722,19 +3877,23 @@
       <c r="D19" s="22">
         <v>249.9</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>237.405</v>
+      </c>
+      <c r="F19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="22">
+      <c r="G19" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>249.9</v>
       </c>
-      <c r="G19" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>12.495000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>237.405</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3747,19 +3906,23 @@
       <c r="D20" s="22">
         <v>259.89999999999998</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="22">
+      <c r="G20" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>0</v>
       </c>
-      <c r="G20" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
+      <c r="H20" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -3772,19 +3935,23 @@
       <c r="D21" s="22">
         <v>259.89999999999998</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>246.90499999999997</v>
+      </c>
+      <c r="F21" s="1">
         <v>1</v>
       </c>
-      <c r="F21" s="22">
+      <c r="G21" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>259.89999999999998</v>
       </c>
-      <c r="G21" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>12.994999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>246.90499999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3797,19 +3964,23 @@
       <c r="D22" s="22">
         <v>39.9</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>37.905000000000001</v>
+      </c>
+      <c r="F22" s="1">
         <v>11</v>
       </c>
-      <c r="F22" s="22">
+      <c r="G22" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>438.9</v>
       </c>
-      <c r="G22" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>21.945</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>416.95500000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3822,41 +3993,49 @@
       <c r="D23" s="22">
         <v>49.9</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="22">
+        <f>Tabela3[[#This Row],[Preço Unitário]]-(Tabela3[[#This Row],[Preço Unitário]]*$J$4)</f>
+        <v>47.405000000000001</v>
+      </c>
+      <c r="F23" s="1">
         <v>21</v>
       </c>
-      <c r="F23" s="22">
+      <c r="G23" s="22">
         <f>Tabela3[[#This Row],[Preço Unitário]]*Tabela3[[#This Row],[Qtde]]</f>
         <v>1047.8999999999999</v>
       </c>
-      <c r="G23" s="29">
-        <f>Tabela3[[#This Row],[Valor Total]]*$I$4</f>
-        <v>52.394999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="29">
+        <f>Tabela3[[#This Row],[Preço C/ Desconto]]*Tabela3[[#This Row],[Qtde]]</f>
+        <v>995.505</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="22">
         <f>SUBTOTAL(109,Tabela3[Preço Unitário])</f>
         <v>2983.0000000000009</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="22">
+        <f>SUBTOTAL(109,Tabela3[Preço C/ Desconto])</f>
+        <v>2833.8500000000004</v>
+      </c>
+      <c r="F24" s="1">
         <f>SUBTOTAL(109,Tabela3[Qtde])</f>
         <v>132</v>
       </c>
-      <c r="F24" s="29">
+      <c r="G24" s="29">
         <f>SUBTOTAL(109,Tabela3[Valor Total])</f>
         <v>10227.799999999999</v>
       </c>
-      <c r="G24" s="29">
-        <f>SUBTOTAL(109,Tabela3[Valor do Desconto])</f>
-        <v>511.39000000000004</v>
+      <c r="H24" s="29">
+        <f>SUBTOTAL(109,Tabela3[Valor Desconto Total])</f>
+        <v>9716.41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>

</xml_diff>